<commit_message>
Move budgets to data provider data
</commit_message>
<xml_diff>
--- a/examples/data/data_provider_example.xlsx
+++ b/examples/data/data_provider_example.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\src\SBTi\examples\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ITR\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
     <sheet name="target_data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="189">
   <si>
     <t>company_name</t>
   </si>
@@ -580,13 +580,25 @@
   </si>
   <si>
     <t>Company AW</t>
+  </si>
+  <si>
+    <t>cumulative_budget</t>
+  </si>
+  <si>
+    <t>cumulative_trajectory</t>
+  </si>
+  <si>
+    <t>cumulative_target</t>
+  </si>
+  <si>
+    <t>target_probability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,9 +675,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q51" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:Q51"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U51" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:U51"/>
+  <tableColumns count="21">
     <tableColumn id="1" name="company_name"/>
     <tableColumn id="2" name="company_id"/>
     <tableColumn id="3" name="isic"/>
@@ -685,6 +697,10 @@
       <calculatedColumnFormula>Table1[[#This Row],[company_market_cap]]*Q2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" name="company_cash_equivalents"/>
+    <tableColumn id="14" name="cumulative_budget"/>
+    <tableColumn id="15" name="cumulative_trajectory"/>
+    <tableColumn id="16" name="cumulative_target"/>
+    <tableColumn id="17" name="target_probability"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -978,13 +994,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I25" workbookViewId="0">
+      <selection activeCell="V39" sqref="V39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -997,7 +1013,7 @@
     <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1049,8 +1065,20 @@
       <c r="Q1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>185</v>
+      </c>
+      <c r="S1" t="s">
+        <v>186</v>
+      </c>
+      <c r="T1" t="s">
+        <v>187</v>
+      </c>
+      <c r="U1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1087,8 +1115,20 @@
       <c r="Q2">
         <v>4528467714.7267609</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>151.28060920540031</v>
+      </c>
+      <c r="S2">
+        <v>335.65335174323133</v>
+      </c>
+      <c r="T2">
+        <v>339.66835709230492</v>
+      </c>
+      <c r="U2">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -1125,8 +1165,20 @@
       <c r="Q3">
         <v>69006940.998092517</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>210.28756399048262</v>
+      </c>
+      <c r="S3">
+        <v>578.79482682229639</v>
+      </c>
+      <c r="T3">
+        <v>472.39883641437115</v>
+      </c>
+      <c r="U3">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -1163,8 +1215,20 @@
       <c r="Q4">
         <v>1163119848.4230556</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>149.1775358970259</v>
+      </c>
+      <c r="S4">
+        <v>519.92594644303142</v>
+      </c>
+      <c r="T4">
+        <v>290.78546460143502</v>
+      </c>
+      <c r="U4">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>170</v>
       </c>
@@ -1201,8 +1265,20 @@
       <c r="Q5">
         <v>117630751.45422383</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>155.81429053755497</v>
+      </c>
+      <c r="S5">
+        <v>586.48563776765798</v>
+      </c>
+      <c r="T5">
+        <v>354.60573060795997</v>
+      </c>
+      <c r="U5">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -1239,8 +1315,20 @@
       <c r="Q6">
         <v>28933197273.168182</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>27.360951439513979</v>
+      </c>
+      <c r="S6">
+        <v>98.757798057827145</v>
+      </c>
+      <c r="T6">
+        <v>105.66095996243746</v>
+      </c>
+      <c r="U6">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -1277,8 +1365,20 @@
       <c r="Q7">
         <v>51876930016.314178</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>320.70129835595458</v>
+      </c>
+      <c r="S7">
+        <v>1016.5298043530278</v>
+      </c>
+      <c r="T7">
+        <v>536.4169776190605</v>
+      </c>
+      <c r="U7">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -1315,8 +1415,20 @@
       <c r="Q8">
         <v>2214490.9702577037</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>49.517672755188094</v>
+      </c>
+      <c r="S8">
+        <v>161.56415575761997</v>
+      </c>
+      <c r="T8">
+        <v>146.41151115367325</v>
+      </c>
+      <c r="U8">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -1353,8 +1465,20 @@
       <c r="Q9">
         <v>203940251.11854151</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>239.18762466646331</v>
+      </c>
+      <c r="S9">
+        <v>697.85352071183479</v>
+      </c>
+      <c r="T9">
+        <v>577.39433075329839</v>
+      </c>
+      <c r="U9">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>175</v>
       </c>
@@ -1391,8 +1515,20 @@
       <c r="Q10">
         <v>42950453116.50563</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>216.75177095667976</v>
+      </c>
+      <c r="S10">
+        <v>430.01617112648546</v>
+      </c>
+      <c r="T10">
+        <v>660.35504275524261</v>
+      </c>
+      <c r="U10">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>176</v>
       </c>
@@ -1429,8 +1565,20 @@
       <c r="Q11">
         <v>5520000408.4878492</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>70.355367219718616</v>
+      </c>
+      <c r="S11">
+        <v>169.8397691123094</v>
+      </c>
+      <c r="T11">
+        <v>143.59484790913928</v>
+      </c>
+      <c r="U11">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -1467,8 +1615,20 @@
       <c r="Q12">
         <v>505519258.45795137</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>155.81902748156233</v>
+      </c>
+      <c r="S12">
+        <v>325.58375119093438</v>
+      </c>
+      <c r="T12">
+        <v>360.04845851784324</v>
+      </c>
+      <c r="U12">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -1505,8 +1665,20 @@
       <c r="Q13">
         <v>462245314.11453331</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>216.59619091019709</v>
+      </c>
+      <c r="S13">
+        <v>561.43098201762746</v>
+      </c>
+      <c r="T13">
+        <v>500.74276659923345</v>
+      </c>
+      <c r="U13">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>179</v>
       </c>
@@ -1543,8 +1715,20 @@
       <c r="Q14">
         <v>1853875026.0311818</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>153.65286197393669</v>
+      </c>
+      <c r="S14">
+        <v>504.32816804974044</v>
+      </c>
+      <c r="T14">
+        <v>308.23259247752117</v>
+      </c>
+      <c r="U14">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -1581,8 +1765,20 @@
       <c r="Q15">
         <v>3272481697.8285317</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>160.48871925368161</v>
+      </c>
+      <c r="S15">
+        <v>568.89106863462825</v>
+      </c>
+      <c r="T15">
+        <v>375.88207444443759</v>
+      </c>
+      <c r="U15">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -1619,8 +1815,20 @@
       <c r="Q16">
         <v>518880676.89759755</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>28.1817799826994</v>
+      </c>
+      <c r="S16">
+        <v>95.795064116092334</v>
+      </c>
+      <c r="T16">
+        <v>112.00061756018371</v>
+      </c>
+      <c r="U16">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
         <v>182</v>
       </c>
@@ -1657,8 +1865,20 @@
       <c r="Q17">
         <v>990719858.47337103</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>330.32233730663324</v>
+      </c>
+      <c r="S17">
+        <v>986.03391022243693</v>
+      </c>
+      <c r="T17">
+        <v>568.6019962762042</v>
+      </c>
+      <c r="U17">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>184</v>
       </c>
@@ -1695,8 +1915,20 @@
       <c r="Q18">
         <v>470283632.88013947</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>51.003202937843739</v>
+      </c>
+      <c r="S18">
+        <v>156.71723108489138</v>
+      </c>
+      <c r="T18">
+        <v>155.19620182289364</v>
+      </c>
+      <c r="U18">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1733,8 +1965,20 @@
       <c r="Q19">
         <v>963039844.50366735</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>246.3632534064572</v>
+      </c>
+      <c r="S19">
+        <v>676.91791509047971</v>
+      </c>
+      <c r="T19">
+        <v>612.03799059849632</v>
+      </c>
+      <c r="U19">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1771,8 +2015,20 @@
       <c r="Q20">
         <v>23467516.32994597</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>223.25432408538018</v>
+      </c>
+      <c r="S20">
+        <v>417.11568599269089</v>
+      </c>
+      <c r="T20">
+        <v>699.97634532055724</v>
+      </c>
+      <c r="U20">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1809,8 +2065,20 @@
       <c r="Q21">
         <v>457926390.7271148</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>72.46602823631018</v>
+      </c>
+      <c r="S21">
+        <v>164.74457603894012</v>
+      </c>
+      <c r="T21">
+        <v>152.21053878368764</v>
+      </c>
+      <c r="U21">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1847,8 +2115,20 @@
       <c r="Q22">
         <v>469617764.24836379</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>160.4935983060092</v>
+      </c>
+      <c r="S22">
+        <v>315.81623865520635</v>
+      </c>
+      <c r="T22">
+        <v>381.65136602891386</v>
+      </c>
+      <c r="U22">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1885,8 +2165,20 @@
       <c r="Q23">
         <v>209706066.63280141</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>223.09407663750301</v>
+      </c>
+      <c r="S23">
+        <v>544.58805255709865</v>
+      </c>
+      <c r="T23">
+        <v>530.78733259518754</v>
+      </c>
+      <c r="U23">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1923,8 +2215,20 @@
       <c r="Q24">
         <v>80140338.552216381</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>158.26244783315479</v>
+      </c>
+      <c r="S24">
+        <v>489.19832300824822</v>
+      </c>
+      <c r="T24">
+        <v>326.72654802617245</v>
+      </c>
+      <c r="U24">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1961,8 +2265,20 @@
       <c r="Q25">
         <v>1863069356.1369269</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>165.30338083129206</v>
+      </c>
+      <c r="S25">
+        <v>551.82433657558943</v>
+      </c>
+      <c r="T25">
+        <v>398.43499891110389</v>
+      </c>
+      <c r="U25">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1999,8 +2315,20 @@
       <c r="Q26">
         <v>802015633.4125073</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>29.027233382180384</v>
+      </c>
+      <c r="S26">
+        <v>92.921212192609559</v>
+      </c>
+      <c r="T26">
+        <v>118.72065461379474</v>
+      </c>
+      <c r="U26">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2037,8 +2365,20 @@
       <c r="Q27">
         <v>1090445581.1975896</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>340.23200742583225</v>
+      </c>
+      <c r="S27">
+        <v>956.45289291576375</v>
+      </c>
+      <c r="T27">
+        <v>602.71811605277651</v>
+      </c>
+      <c r="U27">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -2075,8 +2415,20 @@
       <c r="Q28">
         <v>408632883.32140654</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>52.533299025979055</v>
+      </c>
+      <c r="S28">
+        <v>152.01571415234463</v>
+      </c>
+      <c r="T28">
+        <v>164.50797393226728</v>
+      </c>
+      <c r="U28">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2113,8 +2465,20 @@
       <c r="Q29">
         <v>223357269.54921383</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <v>253.75415100865092</v>
+      </c>
+      <c r="S29">
+        <v>656.61037763776528</v>
+      </c>
+      <c r="T29">
+        <v>648.76027003440618</v>
+      </c>
+      <c r="U29">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -2151,8 +2515,20 @@
       <c r="Q30">
         <v>1279584288.1275206</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <v>229.95195380794158</v>
+      </c>
+      <c r="S30">
+        <v>404.60221541291014</v>
+      </c>
+      <c r="T30">
+        <v>741.97492603979072</v>
+      </c>
+      <c r="U30">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -2189,8 +2565,20 @@
       <c r="Q31">
         <v>259739897.26190066</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <v>74.640009083399491</v>
+      </c>
+      <c r="S31">
+        <v>159.8022387577719</v>
+      </c>
+      <c r="T31">
+        <v>161.34317111070891</v>
+      </c>
+      <c r="U31">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2227,8 +2615,20 @@
       <c r="Q32">
         <v>2957267010.5849843</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <v>165.30840625518948</v>
+      </c>
+      <c r="S32">
+        <v>306.34175149555017</v>
+      </c>
+      <c r="T32">
+        <v>404.55044799064871</v>
+      </c>
+      <c r="U32">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -2265,8 +2665,20 @@
       <c r="Q33">
         <v>3249873922.9934068</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <v>229.78689893662809</v>
+      </c>
+      <c r="S33">
+        <v>528.25041098038571</v>
+      </c>
+      <c r="T33">
+        <v>562.63457255089884</v>
+      </c>
+      <c r="U33">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2303,8 +2715,20 @@
       <c r="Q34">
         <v>1054147392.1400725</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <v>163.01032126814945</v>
+      </c>
+      <c r="S34">
+        <v>474.52237331800075</v>
+      </c>
+      <c r="T34">
+        <v>346.33014090774282</v>
+      </c>
+      <c r="U34">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2341,8 +2765,20 @@
       <c r="Q35">
         <v>16164035.009301951</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <v>170.26248225623084</v>
+      </c>
+      <c r="S35">
+        <v>535.26960647832175</v>
+      </c>
+      <c r="T35">
+        <v>422.34109884577015</v>
+      </c>
+      <c r="U35">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -2379,8 +2815,20 @@
       <c r="Q36">
         <v>76375335.415532187</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36">
+        <v>29.898050383645796</v>
+      </c>
+      <c r="S36">
+        <v>90.133575826831276</v>
+      </c>
+      <c r="T36">
+        <v>125.84389389062243</v>
+      </c>
+      <c r="U36">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -2417,8 +2865,20 @@
       <c r="Q37">
         <v>403556882.32980388</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37">
+        <v>350.43896764860722</v>
+      </c>
+      <c r="S37">
+        <v>927.75930612829086</v>
+      </c>
+      <c r="T37">
+        <v>638.88120301594313</v>
+      </c>
+      <c r="U37">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -2455,8 +2915,20 @@
       <c r="Q38">
         <v>359922992.06079412</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38">
+        <v>54.109297996758428</v>
+      </c>
+      <c r="S38">
+        <v>147.45524272777428</v>
+      </c>
+      <c r="T38">
+        <v>174.37845236820331</v>
+      </c>
+      <c r="U38">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2493,8 +2965,20 @@
       <c r="Q39">
         <v>188775849.06628573</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39">
+        <v>261.36677553891047</v>
+      </c>
+      <c r="S39">
+        <v>636.91206630863235</v>
+      </c>
+      <c r="T39">
+        <v>687.68588623647054</v>
+      </c>
+      <c r="U39">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -2531,8 +3015,20 @@
       <c r="Q40">
         <v>3126017043.1166129</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40">
+        <v>236.85051242217983</v>
+      </c>
+      <c r="S40">
+        <v>392.46414895052283</v>
+      </c>
+      <c r="T40">
+        <v>786.49342160217816</v>
+      </c>
+      <c r="U40">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -2569,8 +3065,20 @@
       <c r="Q41">
         <v>25963862784.153816</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41">
+        <v>76.87920935590148</v>
+      </c>
+      <c r="S41">
+        <v>155.00817159503873</v>
+      </c>
+      <c r="T41">
+        <v>171.02376137735146</v>
+      </c>
+      <c r="U41">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -2607,8 +3115,20 @@
       <c r="Q42">
         <v>216444951.50947747</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42">
+        <v>170.26765844284517</v>
+      </c>
+      <c r="S42">
+        <v>297.15149895068367</v>
+      </c>
+      <c r="T42">
+        <v>428.82347487008764</v>
+      </c>
+      <c r="U42">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -2645,8 +3165,20 @@
       <c r="Q43">
         <v>463981837.16979945</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>236.68050590472694</v>
+      </c>
+      <c r="S43">
+        <v>512.40289865097418</v>
+      </c>
+      <c r="T43">
+        <v>596.39264690395282</v>
+      </c>
+      <c r="U43">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -2683,8 +3215,20 @@
       <c r="Q44">
         <v>630827983.47226107</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>167.90063090619395</v>
+      </c>
+      <c r="S44">
+        <v>460.28670211846071</v>
+      </c>
+      <c r="T44">
+        <v>367.10994936220743</v>
+      </c>
+      <c r="U44">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -2721,8 +3265,20 @@
       <c r="Q45">
         <v>1089931685.5934117</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>175.37035672391778</v>
+      </c>
+      <c r="S45">
+        <v>519.21151828397205</v>
+      </c>
+      <c r="T45">
+        <v>447.68156477651638</v>
+      </c>
+      <c r="U45">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -2759,8 +3315,20 @@
       <c r="Q46">
         <v>1580248549.8247914</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>30.794991895155171</v>
+      </c>
+      <c r="S46">
+        <v>87.429568552026339</v>
+      </c>
+      <c r="T46">
+        <v>133.39452752405978</v>
+      </c>
+      <c r="U46">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47" t="s">
         <v>108</v>
       </c>
@@ -2797,8 +3365,20 @@
       <c r="Q47">
         <v>360167278.93933254</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>360.95213667806547</v>
+      </c>
+      <c r="S47">
+        <v>899.92652694444212</v>
+      </c>
+      <c r="T47">
+        <v>677.21407519689978</v>
+      </c>
+      <c r="U47">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -2835,8 +3415,20 @@
       <c r="Q48">
         <v>23659060554.326973</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>55.732576936661182</v>
+      </c>
+      <c r="S48">
+        <v>143.03158544594103</v>
+      </c>
+      <c r="T48">
+        <v>184.84115951029551</v>
+      </c>
+      <c r="U48">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
       <c r="A49" t="s">
         <v>115</v>
       </c>
@@ -2873,8 +3465,20 @@
       <c r="Q49">
         <v>94976895574.746582</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>269.20777880507779</v>
+      </c>
+      <c r="S49">
+        <v>617.8047043193734</v>
+      </c>
+      <c r="T49">
+        <v>728.94703941065882</v>
+      </c>
+      <c r="U49">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
       <c r="A50" t="s">
         <v>118</v>
       </c>
@@ -2911,8 +3515,20 @@
       <c r="Q50">
         <v>408452279.29417968</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>243.95602779484523</v>
+      </c>
+      <c r="S50">
+        <v>380.69022448200712</v>
+      </c>
+      <c r="T50">
+        <v>833.68302689830887</v>
+      </c>
+      <c r="U50">
+        <v>0.42857142857142849</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
       <c r="A51" t="s">
         <v>183</v>
       </c>
@@ -2948,6 +3564,18 @@
       </c>
       <c r="Q51">
         <v>95987554.945462793</v>
+      </c>
+      <c r="R51">
+        <v>79.185585636578523</v>
+      </c>
+      <c r="S51">
+        <v>150.35792644718757</v>
+      </c>
+      <c r="T51">
+        <v>181.28518705999255</v>
+      </c>
+      <c r="U51">
+        <v>1.4285714285714299</v>
       </c>
     </row>
   </sheetData>
@@ -2963,9 +3591,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -2979,7 +3607,7 @@
     <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3029,7 +3657,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -3070,7 +3698,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -3115,7 +3743,7 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -3156,7 +3784,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>170</v>
       </c>
@@ -3203,7 +3831,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -3250,7 +3878,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -3294,7 +3922,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -3332,7 +3960,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -3376,7 +4004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>175</v>
       </c>
@@ -3420,7 +4048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>176</v>
       </c>
@@ -3464,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -3505,7 +4133,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -3546,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>179</v>
       </c>
@@ -3587,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -3628,7 +4256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -3669,7 +4297,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>182</v>
       </c>
@@ -3710,7 +4338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>184</v>
       </c>
@@ -3748,7 +4376,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3786,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -3824,7 +4452,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3862,7 +4490,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3900,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -3938,7 +4566,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -3979,7 +4607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -4020,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -4061,7 +4689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -4105,7 +4733,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -4140,7 +4768,7 @@
         <v>0.49600000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -4181,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -4222,7 +4850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4263,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4304,7 +4932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -4342,7 +4970,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -4383,7 +5011,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -4418,7 +5046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -4459,7 +5087,7 @@
         <v>6.1699999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -4500,7 +5128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -4541,7 +5169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -4579,7 +5207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -4617,7 +5245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -4661,7 +5289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -4705,7 +5333,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -4746,7 +5374,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>121</v>
       </c>
@@ -4787,7 +5415,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>168</v>
       </c>
@@ -4828,7 +5456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -4872,7 +5500,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -4916,7 +5544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
         <v>171</v>
       </c>
@@ -4957,7 +5585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16">
       <c r="A49" t="s">
         <v>172</v>
       </c>
@@ -5001,7 +5629,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16">
       <c r="A50" t="s">
         <v>173</v>
       </c>
@@ -5048,7 +5676,7 @@
         <v>0.35799999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16">
       <c r="A51" t="s">
         <v>174</v>
       </c>
@@ -5089,7 +5717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16">
       <c r="A52" t="s">
         <v>175</v>
       </c>
@@ -5130,7 +5758,7 @@
         <v>0.32600000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16">
       <c r="A53" t="s">
         <v>176</v>
       </c>
@@ -5174,7 +5802,7 @@
         <v>5.4000000000000006E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16">
       <c r="A54" t="s">
         <v>177</v>
       </c>
@@ -5215,7 +5843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16">
       <c r="A55" t="s">
         <v>178</v>
       </c>
@@ -5256,7 +5884,7 @@
         <v>0.30809999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -5297,7 +5925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16">
       <c r="A57" t="s">
         <v>180</v>
       </c>
@@ -5338,7 +5966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16">
       <c r="A58" t="s">
         <v>181</v>
       </c>
@@ -5379,7 +6007,7 @@
         <v>0.41000000000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16">
       <c r="A59" t="s">
         <v>182</v>
       </c>
@@ -5423,7 +6051,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16">
       <c r="A60" t="s">
         <v>184</v>
       </c>
@@ -5467,7 +6095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16">
       <c r="A61" t="s">
         <v>81</v>
       </c>
@@ -5511,7 +6139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -5552,7 +6180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -5593,7 +6221,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -5634,7 +6262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16">
       <c r="A65" t="s">
         <v>90</v>
       </c>
@@ -5678,7 +6306,7 @@
         <v>0.47789999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -5722,7 +6350,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16">
       <c r="A67" t="s">
         <v>83</v>
       </c>
@@ -5763,7 +6391,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -5807,7 +6435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -5845,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -5886,7 +6514,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -5930,7 +6558,7 @@
         <v>6.4100000000000004E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -5971,7 +6599,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -6012,7 +6640,7 @@
         <v>0.11220000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -6056,7 +6684,7 @@
         <v>0.22870000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -6097,7 +6725,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16">
       <c r="A76" t="s">
         <v>40</v>
       </c>
@@ -6141,7 +6769,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16">
       <c r="A77" t="s">
         <v>43</v>
       </c>
@@ -6185,7 +6813,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16">
       <c r="A78" t="s">
         <v>53</v>
       </c>
@@ -6229,7 +6857,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -6267,7 +6895,7 @@
         <v>0.84400000000000008</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16">
       <c r="A80" t="s">
         <v>168</v>
       </c>
@@ -6314,7 +6942,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -6358,7 +6986,7 @@
         <v>0.55670000000000008</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16">
       <c r="A82" t="s">
         <v>170</v>
       </c>
@@ -6399,7 +7027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16">
       <c r="A83" t="s">
         <v>171</v>
       </c>
@@ -6440,7 +7068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16">
       <c r="A84" t="s">
         <v>172</v>
       </c>
@@ -6481,7 +7109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16">
       <c r="A85" t="s">
         <v>173</v>
       </c>
@@ -6522,7 +7150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16">
       <c r="A86" t="s">
         <v>174</v>
       </c>
@@ -6560,7 +7188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16">
       <c r="A87" t="s">
         <v>175</v>
       </c>
@@ -6604,7 +7232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16">
       <c r="A88" t="s">
         <v>176</v>
       </c>
@@ -6642,7 +7270,7 @@
         <v>0.36700000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16">
       <c r="A89" t="s">
         <v>178</v>
       </c>
@@ -6683,7 +7311,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16">
       <c r="A90" t="s">
         <v>180</v>
       </c>
@@ -6721,7 +7349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -6759,7 +7387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16">
       <c r="A92" t="s">
         <v>181</v>
       </c>
@@ -6797,7 +7425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16">
       <c r="A93" t="s">
         <v>181</v>
       </c>
@@ -6835,7 +7463,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -6876,7 +7504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16">
       <c r="A95" t="s">
         <v>121</v>
       </c>
@@ -6917,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16">
       <c r="A96" t="s">
         <v>168</v>
       </c>
@@ -6961,7 +7589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16">
       <c r="A97" t="s">
         <v>169</v>
       </c>
@@ -7005,7 +7633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16">
       <c r="A98" t="s">
         <v>170</v>
       </c>
@@ -7043,7 +7671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16">
       <c r="A99" t="s">
         <v>170</v>
       </c>
@@ -7081,7 +7709,7 @@
         <v>0.82000000000000006</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16">
       <c r="A100" t="s">
         <v>172</v>
       </c>
@@ -7125,7 +7753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16">
       <c r="A101" t="s">
         <v>173</v>
       </c>
@@ -7163,7 +7791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16">
       <c r="A102" t="s">
         <v>174</v>
       </c>
@@ -7204,7 +7832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16">
       <c r="A103" t="s">
         <v>175</v>
       </c>
@@ -7248,7 +7876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16">
       <c r="A104" t="s">
         <v>176</v>
       </c>
@@ -7292,7 +7920,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16">
       <c r="A105" t="s">
         <v>177</v>
       </c>
@@ -7333,7 +7961,7 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16">
       <c r="A106" t="s">
         <v>178</v>
       </c>
@@ -7377,7 +8005,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16">
       <c r="A107" t="s">
         <v>179</v>
       </c>
@@ -7418,7 +8046,7 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16">
       <c r="A108" t="s">
         <v>180</v>
       </c>
@@ -7459,7 +8087,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16">
       <c r="A109" t="s">
         <v>181</v>
       </c>
@@ -7503,7 +8131,7 @@
         <v>0.57020000000000004</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16">
       <c r="A110" t="s">
         <v>182</v>
       </c>
@@ -7544,7 +8172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16">
       <c r="A111" t="s">
         <v>184</v>
       </c>
@@ -7585,7 +8213,7 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16">
       <c r="A112" t="s">
         <v>83</v>
       </c>
@@ -7626,7 +8254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16">
       <c r="A113" t="s">
         <v>85</v>
       </c>
@@ -7667,7 +8295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16">
       <c r="A114" t="s">
         <v>88</v>
       </c>
@@ -7708,7 +8336,7 @@
         <v>1.52E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16">
       <c r="A115" t="s">
         <v>90</v>
       </c>
@@ -7749,7 +8377,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16">
       <c r="A116" t="s">
         <v>81</v>
       </c>
@@ -7790,7 +8418,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16">
       <c r="A117" t="s">
         <v>83</v>
       </c>
@@ -7834,7 +8462,7 @@
         <v>0.154</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16">
       <c r="A118" t="s">
         <v>83</v>
       </c>
@@ -7878,7 +8506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16">
       <c r="A119" t="s">
         <v>83</v>
       </c>
@@ -7919,7 +8547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16">
       <c r="A120" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
clean up and extra checks
</commit_message>
<xml_diff>
--- a/examples/data/data_provider_example.xlsx
+++ b/examples/data/data_provider_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="184">
   <si>
     <t>company_name</t>
   </si>
@@ -5173,8 +5173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7399,7 +7399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -12414,8 +12414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -21475,6 +21475,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21482,8 +21483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -26561,100 +26562,160 @@
       <c r="A32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>111</v>
+      </c>
+      <c r="B51" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -26668,7 +26729,7 @@
   <dimension ref="A1:AR81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>